<commit_message>
[TAN-6037] Fixed multiple other options
</commit_message>
<xml_diff>
--- a/back/engines/commercial/bulk_import_ideas/spec/fixtures/import_select_other.xlsx
+++ b/back/engines/commercial/bulk_import_ideas/spec/fixtures/import_select_other.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>First name(s)</t>
   </si>
@@ -37,6 +37,12 @@
     <t>Another select field</t>
   </si>
   <si>
+    <t>Third select field</t>
+  </si>
+  <si>
+    <t>Fourth select field</t>
+  </si>
+  <si>
     <t>Bill</t>
   </si>
   <si>
@@ -59,6 +65,12 @@
   </si>
   <si>
     <t>Answer two</t>
+  </si>
+  <si>
+    <t>Answer three</t>
+  </si>
+  <si>
+    <t>Answer Four</t>
   </si>
   <si>
     <t>Bob</t>
@@ -150,10 +162,10 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -312,13 +324,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -416,10 +422,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -665,13 +671,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -973,10 +973,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1218,7 +1218,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1228,11 +1228,11 @@
     <col min="3" max="3" width="14.8516" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.1719" style="1" customWidth="1"/>
     <col min="5" max="5" width="34.6719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.1172" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.9844" style="1" customWidth="1"/>
-    <col min="9" max="9" width="35.1719" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1719" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27" style="1" customWidth="1"/>
+    <col min="9" max="13" width="35.1719" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.6" customHeight="1">
@@ -1263,61 +1263,95 @@
       <c r="I1" t="s" s="2">
         <v>6</v>
       </c>
+      <c r="J1" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" ht="14.6" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s" s="3">
         <v>15</v>
+      </c>
+      <c r="K2" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s" s="3">
+        <v>19</v>
       </c>
     </row>
     <row r="3" ht="14.6" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s" s="3">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" t="s" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I3" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s" s="3">
         <v>15</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="M3" t="s" s="3">
+        <v>19</v>
       </c>
     </row>
     <row r="4" ht="14.6" customHeight="1">
@@ -1330,6 +1364,10 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
     </row>
     <row r="5" ht="14.6" customHeight="1">
       <c r="A5" s="4"/>
@@ -1341,6 +1379,10 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
     </row>
     <row r="6" ht="14.6" customHeight="1">
       <c r="A6" s="4"/>
@@ -1352,6 +1394,10 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
     </row>
     <row r="7" ht="14.6" customHeight="1">
       <c r="A7" s="4"/>
@@ -1363,6 +1409,10 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
     </row>
     <row r="8" ht="14.6" customHeight="1">
       <c r="A8" s="4"/>
@@ -1374,6 +1424,10 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
     </row>
     <row r="9" ht="14.6" customHeight="1">
       <c r="A9" s="4"/>
@@ -1385,6 +1439,10 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
     </row>
     <row r="10" ht="14.6" customHeight="1">
       <c r="A10" s="4"/>
@@ -1396,6 +1454,10 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>